<commit_message>
Modules added to implement code
</commit_message>
<xml_diff>
--- a/testdata/ClaimsCenter.xlsx
+++ b/testdata/ClaimsCenter.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{461A78B2-6017-4A3F-895F-235B46124293}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\training2\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B15CBCF-F959-4554-9A84-739D9C9C9D6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20670" windowHeight="11700" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="3345" windowWidth="15375" windowHeight="7875" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,6 @@
     <sheet name="Invoice" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="168">
   <si>
     <t>TD_UserName</t>
   </si>
@@ -499,9 +503,6 @@
     <t>70088</t>
   </si>
   <si>
-    <t>Claimant</t>
-  </si>
-  <si>
     <t>Lakshmi</t>
   </si>
   <si>
@@ -524,6 +525,18 @@
   </si>
   <si>
     <t>Auto1 - TeamA</t>
+  </si>
+  <si>
+    <t>04/08/2021</t>
+  </si>
+  <si>
+    <t>InsuredName</t>
+  </si>
+  <si>
+    <t>Akash Gowda</t>
+  </si>
+  <si>
+    <t>Self/Insured</t>
   </si>
 </sst>
 </file>
@@ -620,7 +633,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -669,12 +682,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -791,6 +815,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1532,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAC3BBF-B3BA-44D1-A41A-B54909BFA2EB}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,9 +1582,10 @@
     <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -1603,8 +1634,11 @@
       <c r="P1" s="35" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="44" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>98</v>
       </c>
@@ -1651,10 +1685,13 @@
         <v>155</v>
       </c>
       <c r="P2" s="34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>128</v>
       </c>
@@ -1662,10 +1699,10 @@
         <v>144</v>
       </c>
       <c r="C3" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>157</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>158</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>147</v>
@@ -1701,7 +1738,7 @@
         <v>155</v>
       </c>
       <c r="P3" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1717,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6534BE01-4C47-4EFD-985F-408E3EBD759A}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,11 +1816,11 @@
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="20">
-        <v>5850681293</v>
+        <v>7026684222</v>
       </c>
       <c r="F2" s="30"/>
       <c r="G2" s="25" t="s">
-        <v>100</v>
+        <v>164</v>
       </c>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
@@ -1843,13 +1880,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="41" t="s">
         <v>161</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,10 +1894,10 @@
         <v>98</v>
       </c>
       <c r="B2" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="34" t="s">
         <v>163</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>164</v>
       </c>
       <c r="D2" s="43" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Claims TestCases Updated fnol
</commit_message>
<xml_diff>
--- a/testdata/ClaimsCenter.xlsx
+++ b/testdata/ClaimsCenter.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E04A98BD-4AE6-4687-BA07-8D63A3F7DA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash Gowda\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC1\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385CD5AD-18A3-4A16-ABE6-3AC76ADCB140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19680" windowHeight="11760" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -28,8 +33,7 @@
     <sheet name="recovery" sheetId="17" r:id="rId18"/>
     <sheet name="Invoice" sheetId="4" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <oleSize ref="A1:N15"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="235">
   <si>
     <t>gw</t>
   </si>
@@ -596,9 +600,6 @@
     <t>Indiana</t>
   </si>
   <si>
-    <t>343-34-3478</t>
-  </si>
-  <si>
     <t>WhatHappened</t>
   </si>
   <si>
@@ -702,6 +703,51 @@
   </si>
   <si>
     <t>PickupLocation</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_VerifiedPolicy_PartiesInvolved_Contacts</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_VerifiedPolicy_PartiesInvolved_DuplicateContactsVerify</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_VerifiedPolicy_NewExposure_MedicalPayments</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_VerifiedPolicy_AddingReserve</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_VerifiedPolicy_ManualAdjusterCheck_Create</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_VerifiedPolicy_Recovery_CreateRecovery</t>
+  </si>
+  <si>
+    <t>000-00-000635</t>
+  </si>
+  <si>
+    <t>000-00-000643</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>000-00-000651</t>
+  </si>
+  <si>
+    <t>345-34-353</t>
+  </si>
+  <si>
+    <t>345-34-300</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_UnverifiedPolicy_Newclaim_Auto_SelectPolicy</t>
+  </si>
+  <si>
+    <t>000-00-000724</t>
+  </si>
+  <si>
+    <t>8306305845</t>
   </si>
 </sst>
 </file>
@@ -819,7 +865,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -879,12 +925,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -922,7 +981,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -983,9 +1041,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1014,6 +1069,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1295,47 +1364,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>142</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1352,10 +1421,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="41" t="s">
         <v>142</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1375,7 +1444,7 @@
       <c r="A4" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="40" t="s">
         <v>142</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1395,7 +1464,7 @@
       <c r="A5" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="41" t="s">
         <v>142</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1411,11 +1480,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1431,11 +1500,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B7" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>142</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1451,11 +1520,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B8" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>142</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1471,21 +1540,161 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+    <row r="9" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1504,47 +1713,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1578,28 +1787,28 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B9A1A7-4849-4AFC-A8A1-F64606261CAE}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>202</v>
+      <c r="B1" s="35" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -1607,7 +1816,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
       <c r="B3" t="s">
@@ -1630,32 +1839,88 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>161</v>
+        <v>220</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>163</v>
+        <v>222</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="13"/>
+    <row r="9" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1672,12 +1937,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="11.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="9" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,35 +2021,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67046DC7-4611-49B8-8755-949DBC7B1CFA}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>209</v>
+      <c r="B1" s="35" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="45">
         <v>1861865084</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="46" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>234</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1794,46 +2063,46 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CE2E52-78BF-40AA-BD5D-501AE9A2E176}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1864,7 +2133,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -1886,6 +2155,58 @@
         <v>126</v>
       </c>
       <c r="H3" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1896,32 +2217,32 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D98CCE47-0C4B-444D-90C2-007C900582DC}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>204</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,7 +2260,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -1949,6 +2270,20 @@
         <v>144</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1959,51 +2294,59 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47936DC1-1333-4359-AF5E-3E7BA7271D6A}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="D1" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="H1" s="36" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>114</v>
       </c>
@@ -2013,24 +2356,24 @@
       <c r="C2" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>200</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -2039,55 +2382,85 @@
       <c r="C3" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="13">
+      <c r="H3" s="13">
         <v>200</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="I3" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="J3" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="13">
+        <v>200</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>135</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1B16E0-B3FA-48B0-9C2B-975E0CBC355F}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>207</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2108,16 +2481,30 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="47">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="47">
         <v>200</v>
       </c>
     </row>
@@ -2128,43 +2515,51 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00227C49-AC2E-48E8-8988-19C7BF9DF3BF}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="D1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>114</v>
       </c>
@@ -2174,18 +2569,18 @@
       <c r="C2" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="13">
+      <c r="H2" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -2194,13 +2589,36 @@
       <c r="C3" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="13">
+      <c r="H3" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="13">
         <v>5</v>
       </c>
     </row>
@@ -2219,8 +2637,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2253,28 +2671,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D031204-5B95-4D59-A8D1-057F094D5E73}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
       <c r="B2" t="s">
@@ -2282,7 +2700,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
       <c r="B3" t="s">
@@ -2299,18 +2717,68 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7"/>
+    </row>
+    <row r="8" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="13" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2329,13 +2797,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2436,256 +2904,255 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0D1CEF-B266-4241-89A5-652CE19CAC48}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="17" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" style="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="25"/>
-    <col min="20" max="20" width="11.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.28515625" style="25" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8" style="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15" style="25" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="34.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="25"/>
-    <col min="30" max="30" width="11.42578125" style="25" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12" style="25" bestFit="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="69.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="20" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.5703125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.140625" style="24" collapsed="1"/>
+    <col min="20" max="20" width="11.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.5703125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="34.5703125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="9.140625" style="24" collapsed="1"/>
+    <col min="30" max="30" width="11.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.5703125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="8.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="16384" width="9.140625" style="24" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="45" t="s">
+      <c r="B1" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="46" t="s">
+      <c r="O1" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="35" t="s">
+      <c r="Q1" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="S1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="35" t="s">
+      <c r="U1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="35" t="s">
+      <c r="V1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="W1" s="35" t="s">
+      <c r="W1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="35" t="s">
+      <c r="X1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" s="35" t="s">
+      <c r="Y1" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="Z1" s="35" t="s">
+      <c r="Z1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="AA1" s="35" t="s">
+      <c r="AA1" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="35" t="s">
+      <c r="AB1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="AC1" s="35" t="s">
+      <c r="AC1" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="35" t="s">
+      <c r="AD1" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="AE1" s="35" t="s">
+      <c r="AE1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="AF1" s="35" t="s">
+      <c r="AF1" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="AG1" s="35" t="s">
+      <c r="AG1" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="AH1" s="35" t="s">
+      <c r="AH1" s="34" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>126</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="25">
         <v>10</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="O2" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26" t="s">
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="27" t="s">
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="AB2" s="26" t="s">
+      <c r="AB2" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="AC2" s="26" t="s">
+      <c r="AC2" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="AD2" s="26" t="s">
+      <c r="AD2" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="AE2" s="26" t="s">
+      <c r="AE2" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="AF2" s="26" t="s">
+      <c r="AF2" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="AG2" s="27" t="s">
+      <c r="AG2" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="AH2" s="26" t="s">
+      <c r="AH2" s="25" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>126</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="26" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2693,46 +3160,183 @@
       <c r="A4" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>117</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="5" t="s">
         <v>166</v>
+      </c>
+      <c r="F6" s="55" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>162</v>
+        <v>221</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F7" s="55" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2744,144 +3348,144 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAC3BBF-B3BA-44D1-A41A-B54909BFA2EB}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="44" t="s">
+      <c r="R1" s="42" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="P2" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="23" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2898,18 +3502,53 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="13" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2924,99 +3563,99 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6534BE01-4C47-4EFD-985F-408E3EBD759A}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="31.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="13.140625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="13.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="F1" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="F1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="O1" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="S1" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="35" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="14" t="s">
@@ -3025,23 +3664,23 @@
       <c r="C2" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="E2" s="40">
-        <f t="shared" ref="E2:E8" ca="1" si="0">TODAY()</f>
-        <v>44350</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="14"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
+      <c r="E2" s="57">
+        <f t="shared" ref="E2:F15" ca="1" si="0">TODAY()</f>
+        <v>44351</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -3050,23 +3689,29 @@
       <c r="C3" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44350</v>
-      </c>
-      <c r="F3" s="39">
+        <v>44351</v>
+      </c>
+      <c r="F3" s="60">
         <f ca="1">TODAY()</f>
-        <v>44350</v>
-      </c>
-      <c r="G3" s="39">
+        <v>44351</v>
+      </c>
+      <c r="G3" s="60">
         <v>44696</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>144</v>
       </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -3081,12 +3726,21 @@
       <c r="D4" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>44351</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>150</v>
       </c>
@@ -3096,17 +3750,26 @@
       <c r="C5" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>5709994140</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44350</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>44351</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>161</v>
+        <v>220</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>77</v>
@@ -3114,156 +3777,395 @@
       <c r="C6" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D6">
-        <v>5709994140</v>
-      </c>
-      <c r="E6" s="39">
+      <c r="D6" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44350</v>
-      </c>
-      <c r="F6" s="39">
-        <f ca="1">TODAY()</f>
-        <v>44350</v>
-      </c>
-      <c r="G6" s="39">
+        <v>44351</v>
+      </c>
+      <c r="F6" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="G6" s="60">
         <v>44696</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="O6" s="13">
-        <v>46074</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" s="13">
-        <v>5709994140</v>
-      </c>
-      <c r="E7" s="39">
+        <v>143</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44350</v>
-      </c>
-      <c r="F7" s="39">
-        <v>44197</v>
-      </c>
-      <c r="G7" s="39">
-        <v>44562</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="O7" s="13">
-        <v>46074</v>
-      </c>
-      <c r="P7" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>174</v>
-      </c>
-      <c r="R7">
-        <v>2015</v>
-      </c>
-      <c r="S7" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="T7" s="54">
-        <v>10000</v>
-      </c>
-      <c r="U7" s="53">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>44351</v>
+      </c>
+      <c r="F7" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="G7" s="60">
+        <v>44696</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>163</v>
+        <v>222</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="F8" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="G8" s="60">
+        <v>44696</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="F9" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="G9" s="60">
+        <v>44696</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="F10" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="G10" s="60">
+        <v>44696</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="F11" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="G11" s="60">
+        <v>44696</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="5">
+        <v>5709994140</v>
+      </c>
+      <c r="E12" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="F12" s="60">
+        <f ca="1">TODAY()</f>
+        <v>44351</v>
+      </c>
+      <c r="G12" s="60">
+        <v>44696</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="O12" s="13">
+        <v>46074</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5709994140</v>
+      </c>
+      <c r="E13" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="F13" s="60">
+        <f ca="1">TODAY()</f>
+        <v>44351</v>
+      </c>
+      <c r="G13" s="60">
+        <v>44696</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="O13" s="13">
+        <v>46074</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5709994140</v>
+      </c>
+      <c r="E14" s="60">
+        <f t="shared" ca="1" si="0"/>
+        <v>44351</v>
+      </c>
+      <c r="F14" s="60">
+        <v>44197</v>
+      </c>
+      <c r="G14" s="60">
+        <v>44562</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="O14" s="13">
+        <v>46074</v>
+      </c>
+      <c r="P14" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>174</v>
+      </c>
+      <c r="R14">
+        <v>2015</v>
+      </c>
+      <c r="S14" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="T14" s="52">
+        <v>10000</v>
+      </c>
+      <c r="U14" s="51">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D8">
+      <c r="D15" s="5">
         <v>5709994140</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E15" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44350</v>
-      </c>
-      <c r="F8" s="39">
+        <v>44351</v>
+      </c>
+      <c r="F15" s="60">
         <f ca="1">TODAY()</f>
-        <v>44350</v>
-      </c>
-      <c r="G8" s="39">
+        <v>44351</v>
+      </c>
+      <c r="G15" s="60">
         <v>44696</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13" t="s">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J15" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K15" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L15" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M15" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="N8" s="13" t="s">
+      <c r="N15" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O15" s="13">
         <v>46074</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="50"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3275,82 +4177,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C4E6E2-AAC9-4B7B-B879-C23DF8988E6C}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" style="13" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21" style="13" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="O1" s="35" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3373,8 +4275,8 @@
       <c r="F4" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="G4" s="52" t="s">
-        <v>185</v>
+      <c r="G4" s="50" t="s">
+        <v>230</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>14</v>
@@ -3384,6 +4286,21 @@
       </c>
       <c r="J4" t="s">
         <v>126</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="O4" s="13">
+        <v>46074</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -3430,8 +4347,8 @@
       <c r="F7" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="G7" s="52" t="s">
-        <v>185</v>
+      <c r="G7" s="50" t="s">
+        <v>230</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>14</v>
@@ -3494,32 +4411,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="56"/>
+      <c r="B2" s="54"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3532,7 +4449,7 @@
       <c r="A5" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="54" t="s">
         <v>117</v>
       </c>
       <c r="C5" s="13" t="s">
@@ -3556,7 +4473,7 @@
       <c r="A8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="54" t="s">
         <v>117</v>
       </c>
       <c r="C8" s="13" t="s">
@@ -3574,72 +4491,72 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBAA54D-4167-4FED-9056-FD7F72E35B94}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="G1" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="G1" s="38" t="s">
-        <v>220</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>147</v>
       </c>
       <c r="B2" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="38">
         <f ca="1">TODAY()</f>
-        <v>44350</v>
-      </c>
-      <c r="D2" s="39">
+        <v>44351</v>
+      </c>
+      <c r="D2" s="38">
         <v>44706</v>
       </c>
-      <c r="E2" s="41">
+      <c r="E2" s="39">
         <v>10</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="36" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3653,18 +4570,53 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="13" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Claims Updated version 8
</commit_message>
<xml_diff>
--- a/testdata/ClaimsCenter.xlsx
+++ b/testdata/ClaimsCenter.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labor\git\blackcomb\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash Gowda\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515D143B-D44F-4411-BD2B-1745E66D827D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1A1DBA-6D45-4C86-BB3D-84EB6461BFA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28065" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19680" windowHeight="11760" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,9 @@
     <sheet name="recovery" sheetId="17" r:id="rId18"/>
     <sheet name="Invoice" sheetId="4" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="243">
   <si>
     <t>gw</t>
   </si>
@@ -769,9 +769,6 @@
   </si>
   <si>
     <t>elUHETasB Automation</t>
-  </si>
-  <si>
-    <t>0389028146</t>
   </si>
   <si>
     <t>0740946203</t>
@@ -1425,12 +1422,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1766,10 +1763,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="66.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1848,8 +1845,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1990,12 +1987,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="9" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="9" width="16.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="9" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="9" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="9" width="14.0" collapsed="true"/>
-    <col min="6" max="16384" style="9" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" style="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="9" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2080,8 +2077,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="61.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2116,21 +2113,21 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CE2E52-78BF-40AA-BD5D-501AE9A2E176}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2211,9 +2208,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>220</v>
+    <row r="4" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>148</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>123</v>
@@ -2234,12 +2231,12 @@
         <v>126</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>231</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>123</v>
@@ -2260,6 +2257,32 @@
         <v>126</v>
       </c>
       <c r="H5" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2278,10 +2301,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="62.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2353,16 +2376,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="59.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="11.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="12.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="1" max="1" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2494,10 +2517,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="46.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2574,14 +2597,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="13" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="12.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2688,8 +2711,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2724,25 +2747,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D031204-5B95-4D59-A8D1-057F094D5E73}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2793,13 +2816,12 @@
       <c r="B2" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="C2"/>
       <c r="D2" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="60" t="n">
+      <c r="E2" s="60">
         <f t="shared" ref="E2:E15" ca="1" si="0">TODAY()</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F2" s="61" t="s">
         <v>241</v>
@@ -2807,11 +2829,9 @@
       <c r="G2" s="62">
         <v>8439809129</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="J2"/>
       <c r="K2" t="s">
         <v>140</v>
       </c>
@@ -2826,14 +2846,12 @@
       <c r="A3" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
       <c r="D3" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="60" t="n">
+      <c r="E3" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F3" s="61" t="s">
         <v>241</v>
@@ -2841,11 +2859,9 @@
       <c r="G3" s="62">
         <v>8439809129</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="J3"/>
       <c r="K3" t="s">
         <v>146</v>
       </c>
@@ -2860,14 +2876,12 @@
       <c r="A4" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B4"/>
-      <c r="C4"/>
       <c r="D4" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="60" t="n">
+      <c r="E4" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F4" s="61" t="s">
         <v>241</v>
@@ -2875,12 +2889,9 @@
       <c r="G4" s="62">
         <v>8439809129</v>
       </c>
-      <c r="H4"/>
       <c r="I4" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
       <c r="L4" s="63" t="s">
         <v>69</v>
       </c>
@@ -2892,14 +2903,12 @@
       <c r="A5" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B5"/>
-      <c r="C5"/>
       <c r="D5" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="60" t="n">
+      <c r="E5" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F5" s="61" t="s">
         <v>241</v>
@@ -2907,12 +2916,9 @@
       <c r="G5" s="62">
         <v>8439809129</v>
       </c>
-      <c r="H5"/>
       <c r="I5" s="62">
         <v>5709994140</v>
       </c>
-      <c r="J5"/>
-      <c r="K5"/>
       <c r="L5" s="63" t="s">
         <v>69</v>
       </c>
@@ -2929,9 +2935,9 @@
       <c r="D6" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="60" t="n">
+      <c r="E6" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F6" s="61" t="s">
         <v>241</v>
@@ -2963,9 +2969,9 @@
       <c r="D7" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="60" t="n">
+      <c r="E7" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F7" s="61" t="s">
         <v>241</v>
@@ -2995,9 +3001,9 @@
       <c r="D8" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="60" t="n">
+      <c r="E8" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F8" s="61" t="s">
         <v>241</v>
@@ -3029,9 +3035,9 @@
       <c r="D9" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="60" t="n">
+      <c r="E9" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F9" s="61" t="s">
         <v>241</v>
@@ -3061,9 +3067,9 @@
       <c r="D10" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="60" t="n">
+      <c r="E10" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F10" s="61" t="s">
         <v>241</v>
@@ -3095,9 +3101,9 @@
       <c r="D11" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="60" t="n">
+      <c r="E11" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F11" s="61" t="s">
         <v>241</v>
@@ -3122,14 +3128,12 @@
       <c r="A12" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B12"/>
-      <c r="C12"/>
       <c r="D12" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="60" t="n">
+      <c r="E12" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F12" s="61" t="s">
         <v>241</v>
@@ -3137,12 +3141,9 @@
       <c r="G12" s="62">
         <v>8439809129</v>
       </c>
-      <c r="H12"/>
       <c r="I12" s="62">
         <v>5709994140</v>
       </c>
-      <c r="J12"/>
-      <c r="K12"/>
       <c r="L12" s="63" t="s">
         <v>69</v>
       </c>
@@ -3159,9 +3160,9 @@
       <c r="D13" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E13" s="60" t="n">
+      <c r="E13" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F13" s="61" t="s">
         <v>241</v>
@@ -3188,14 +3189,12 @@
       <c r="A14" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B14"/>
-      <c r="C14"/>
       <c r="D14" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="60" t="n">
+      <c r="E14" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F14" s="61" t="s">
         <v>241</v>
@@ -3203,12 +3202,9 @@
       <c r="G14" s="62">
         <v>8439809129</v>
       </c>
-      <c r="H14"/>
       <c r="I14" s="62">
         <v>5709994140</v>
       </c>
-      <c r="J14"/>
-      <c r="K14"/>
       <c r="L14" s="63" t="s">
         <v>69</v>
       </c>
@@ -3220,14 +3216,12 @@
       <c r="A15" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B15"/>
-      <c r="C15"/>
       <c r="D15" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="60" t="n">
+      <c r="E15" s="60">
         <f t="shared" ca="1" si="0"/>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F15" s="61" t="s">
         <v>241</v>
@@ -3235,12 +3229,9 @@
       <c r="G15" s="62">
         <v>8439809129</v>
       </c>
-      <c r="H15"/>
       <c r="I15" s="62">
         <v>5709994140</v>
       </c>
-      <c r="J15"/>
-      <c r="K15"/>
       <c r="L15" s="63" t="s">
         <v>69</v>
       </c>
@@ -3263,13 +3254,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3378,40 +3369,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="24" width="69.85546875" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="24" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="24" width="6.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="24" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="24" width="17.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="24" width="29.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="24" width="27.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="24" width="19.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="24" width="26.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="24" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="24" width="9.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="24" width="15.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="24" width="20.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="24" width="11.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="24" width="26.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="24" width="18.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="24" width="21.140625" collapsed="true"/>
-    <col min="19" max="19" style="24" width="9.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="24" width="11.42578125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="24" width="13.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="24" width="11.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="24" width="8.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="24" width="12.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="24" width="34.5703125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="24" width="12.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="24" width="16.7109375" collapsed="true"/>
-    <col min="29" max="29" style="24" width="9.140625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="24" width="11.42578125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="24" width="9.85546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="24" width="9.5703125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="24" width="8.140625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="24" width="12.0" collapsed="true"/>
-    <col min="35" max="16384" style="24" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="20" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="6.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.5703125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.140625" style="24" collapsed="1"/>
+    <col min="20" max="20" width="11.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="8" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.5703125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="34.5703125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="12.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="16.7109375" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="9.140625" style="24" collapsed="1"/>
+    <col min="30" max="30" width="11.42578125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="9.85546875" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.5703125" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="8.140625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="12" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="16384" width="9.140625" style="24" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -3822,20 +3813,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="13" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -4032,27 +4023,27 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="13" width="24.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="13" width="13.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="13" width="31.42578125" collapsed="true"/>
-    <col min="12" max="15" customWidth="true" style="13" width="13.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.42578125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="13.140625" style="13" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -4134,9 +4125,9 @@
       <c r="D2" s="33">
         <v>1075150626</v>
       </c>
-      <c r="E2" s="57" t="n">
+      <c r="E2" s="57">
         <f ca="1">searchValues!E2</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F2" s="57"/>
       <c r="G2" s="57"/>
@@ -4157,16 +4148,17 @@
       <c r="C3" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" s="57" t="n">
+      <c r="D3" s="33" t="str">
+        <f>searchValues!I3</f>
+        <v>9713820364</v>
+      </c>
+      <c r="E3" s="57">
         <f ca="1">searchValues!E3</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F3" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F3" s="57">
         <f ca="1">searchValues!E3</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G3" s="57">
         <v>44696</v>
@@ -4195,9 +4187,9 @@
       <c r="D4" s="33">
         <v>7535227641</v>
       </c>
-      <c r="E4" s="57" t="n">
+      <c r="E4" s="57">
         <f ca="1">searchValues!E4</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F4" s="57"/>
       <c r="G4" s="57"/>
@@ -4223,13 +4215,13 @@
       <c r="D5" s="33">
         <v>1686560131</v>
       </c>
-      <c r="E5" s="57" t="n">
+      <c r="E5" s="57">
         <f ca="1">searchValues!E5</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F5" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F5" s="57">
         <f ca="1">searchValues!E5</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G5" s="57"/>
       <c r="H5" s="5"/>
@@ -4254,13 +4246,13 @@
       <c r="D6" s="33">
         <v>9564477390</v>
       </c>
-      <c r="E6" s="57" t="n">
+      <c r="E6" s="57">
         <f ca="1">searchValues!E6</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F6" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F6" s="57">
         <f ca="1">searchValues!E6</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G6" s="57">
         <v>44696</v>
@@ -4287,13 +4279,13 @@
       <c r="D7" s="33">
         <v>2011697620</v>
       </c>
-      <c r="E7" s="57" t="n">
+      <c r="E7" s="57">
         <f ca="1">searchValues!E7</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F7" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F7" s="57">
         <f ca="1">searchValues!E7</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G7" s="57">
         <v>44696</v>
@@ -4320,13 +4312,13 @@
       <c r="D8" s="33">
         <v>3941875192</v>
       </c>
-      <c r="E8" s="57" t="n">
+      <c r="E8" s="57">
         <f ca="1">searchValues!E8</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F8" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F8" s="57">
         <f ca="1">searchValues!E8</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G8" s="57">
         <v>44696</v>
@@ -4353,13 +4345,13 @@
       <c r="D9" s="33">
         <v>4086806378</v>
       </c>
-      <c r="E9" s="57" t="n">
+      <c r="E9" s="57">
         <f ca="1">searchValues!E9</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F9" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F9" s="57">
         <f ca="1">searchValues!E9</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G9" s="57">
         <v>44696</v>
@@ -4386,13 +4378,13 @@
       <c r="D10" s="33">
         <v>4030439314</v>
       </c>
-      <c r="E10" s="57" t="n">
+      <c r="E10" s="57">
         <f ca="1">searchValues!E10</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F10" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F10" s="57">
         <f ca="1">searchValues!E10</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G10" s="57">
         <v>44696</v>
@@ -4419,13 +4411,13 @@
       <c r="D11" s="33">
         <v>5012031479</v>
       </c>
-      <c r="E11" s="57" t="n">
+      <c r="E11" s="57">
         <f ca="1">searchValues!E11</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F11" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F11" s="57">
         <f ca="1">searchValues!E11</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G11" s="57">
         <v>44696</v>
@@ -4452,13 +4444,13 @@
       <c r="D12" s="33">
         <v>1272770452</v>
       </c>
-      <c r="E12" s="57" t="n">
+      <c r="E12" s="57">
         <f ca="1">searchValues!E12</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F12" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F12" s="57">
         <f ca="1">searchValues!E12</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G12" s="57">
         <v>44696</v>
@@ -4500,13 +4492,13 @@
       <c r="D13" s="33">
         <v>4172446499</v>
       </c>
-      <c r="E13" s="57" t="n">
+      <c r="E13" s="57">
         <f ca="1">searchValues!E13</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F13" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F13" s="57">
         <f ca="1">searchValues!E13</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G13" s="57">
         <v>44696</v>
@@ -4546,11 +4538,11 @@
         <v>164</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>243</v>
-      </c>
-      <c r="E14" s="57" t="n">
+        <v>242</v>
+      </c>
+      <c r="E14" s="57">
         <f ca="1">searchValues!E14</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="F14" s="57">
         <v>44197</v>
@@ -4610,17 +4602,17 @@
       <c r="C15" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="D15" s="33" t="n">
+      <c r="D15" s="33">
         <f>searchValues!I15</f>
-        <v>5.70999414E9</v>
-      </c>
-      <c r="E15" s="57" t="n">
+        <v>5709994140</v>
+      </c>
+      <c r="E15" s="57">
         <f ca="1">searchValues!E15</f>
-        <v>44355.0</v>
-      </c>
-      <c r="F15" s="57" t="n">
+        <v>44355</v>
+      </c>
+      <c r="F15" s="57">
         <f ca="1">searchValues!E15</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="G15" s="57">
         <v>44696</v>
@@ -4667,18 +4659,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="66.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="13" width="18.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="13" width="21.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="13" width="21.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.28515625" style="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21" style="13" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -4895,8 +4887,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="66.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4983,13 +4975,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5022,9 +5014,9 @@
       <c r="B2" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="38" t="n">
+      <c r="C2" s="38">
         <f ca="1">TODAY()</f>
-        <v>44355.0</v>
+        <v>44355</v>
       </c>
       <c r="D2" s="38">
         <v>44706</v>

</xml_diff>

<commit_message>
ClaimsAssignClaim Scripting in progress
</commit_message>
<xml_diff>
--- a/testdata/ClaimsCenter.xlsx
+++ b/testdata/ClaimsCenter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\agowda\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash Gowda\git\AUT_FW_SEL_JAVA_GW_CM_BC_PC_CC\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD7D19A-522E-49CC-AEFB-FE2C536AF447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FB1068-5E35-4AE0-A9AE-3C9B8FC9163E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19680" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -32,27 +32,19 @@
     <sheet name="reserves" sheetId="16" r:id="rId17"/>
     <sheet name="recovery" sheetId="17" r:id="rId18"/>
     <sheet name="UploadDocuments" sheetId="21" r:id="rId19"/>
+    <sheet name="AssignClaim" sheetId="24" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="254">
   <si>
     <t>gw</t>
   </si>
@@ -793,6 +785,27 @@
   </si>
   <si>
     <t>345-34-310</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_VerifiedPolicy_AssignClaim_RoundRobin_LoadFactor100</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1366 Pine Valley Rd, Alaska, CA</t>
+  </si>
+  <si>
+    <t>AUT_PA_CC_FNOL_VerifiedPolicy_AutomatedAssignclaim</t>
+  </si>
+  <si>
+    <t>Vendor (Company)</t>
+  </si>
+  <si>
+    <t>SearchAddressBookType</t>
+  </si>
+  <si>
+    <t>SearchAddressBookName</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1169,6 +1182,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1450,20 +1466,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1488,7 +1504,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>121</v>
@@ -1883,6 +1899,26 @@
         <v>95</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1895,18 +1931,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CA2C57-AFEC-4504-AC59-9C52C5077376}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="66.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1925,7 +1961,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>83</v>
@@ -2033,6 +2069,11 @@
     <row r="21" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2042,16 +2083,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B9A1A7-4849-4AFC-A8A1-F64606261CAE}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2064,7 +2105,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>99</v>
@@ -2219,6 +2260,14 @@
         <v>239</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2237,12 +2286,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="6" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="16.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="6" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="6" width="14.0" collapsed="true"/>
-    <col min="6" max="16384" style="6" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" style="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="6" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2327,8 +2376,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="61.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="61.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2371,13 +2420,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2794,17 +2843,17 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3125,17 +3174,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="62" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="62" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="62" width="72.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="62" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="62" width="12.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="62" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="62" width="16.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="62" width="16.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="62" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="62" width="11.42578125" collapsed="true"/>
-    <col min="11" max="16384" style="62" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="72.140625" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.85546875" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.140625" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" style="62" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="16384" width="9.140625" style="62" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3790,12 +3839,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="57" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="57" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="57" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="57" width="21.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="57" width="1.85546875" collapsed="true"/>
-    <col min="6" max="16384" style="57" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" style="57" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" style="57" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.7109375" style="57" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.85546875" style="57" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="1.85546875" style="57" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="57" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4026,14 +4075,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="12.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4387,11 +4436,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="10" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4578,27 +4627,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D031204-5B95-4D59-A8D1-057F094D5E73}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4644,18 +4693,17 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="C2"/>
       <c r="D2" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="50" t="n">
+      <c r="E2" s="50">
         <f t="shared" ref="E2:E17" ca="1" si="0">TODAY()</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F2" s="51" t="s">
         <v>219</v>
@@ -4663,11 +4711,9 @@
       <c r="G2" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H2"/>
       <c r="I2" s="52">
         <v>9849450932</v>
       </c>
-      <c r="J2"/>
       <c r="K2" t="s">
         <v>119</v>
       </c>
@@ -4682,14 +4728,12 @@
       <c r="A3" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="B3"/>
-      <c r="C3"/>
       <c r="D3" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="50" t="n">
+      <c r="E3" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F3" s="51" t="s">
         <v>219</v>
@@ -4697,11 +4741,9 @@
       <c r="G3" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H3"/>
       <c r="I3" s="52">
         <v>9849450932</v>
       </c>
-      <c r="J3"/>
       <c r="K3" t="s">
         <v>125</v>
       </c>
@@ -4716,14 +4758,12 @@
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B4"/>
-      <c r="C4"/>
       <c r="D4" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="50" t="n">
+      <c r="E4" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F4" s="51" t="s">
         <v>219</v>
@@ -4731,12 +4771,9 @@
       <c r="G4" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H4"/>
       <c r="I4" s="52">
         <v>9849450932</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
       <c r="L4" s="53" t="s">
         <v>51</v>
       </c>
@@ -4748,14 +4785,12 @@
       <c r="A5" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B5"/>
-      <c r="C5"/>
       <c r="D5" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="50" t="n">
+      <c r="E5" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F5" s="51" t="s">
         <v>219</v>
@@ -4763,12 +4798,9 @@
       <c r="G5" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H5"/>
       <c r="I5" s="52">
         <v>9849450932</v>
       </c>
-      <c r="J5"/>
-      <c r="K5"/>
       <c r="L5" s="53" t="s">
         <v>51</v>
       </c>
@@ -4785,9 +4817,9 @@
       <c r="D6" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="50" t="n">
+      <c r="E6" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F6" s="51" t="s">
         <v>219</v>
@@ -4819,9 +4851,9 @@
       <c r="D7" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="50" t="n">
+      <c r="E7" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F7" s="51" t="s">
         <v>219</v>
@@ -4851,9 +4883,9 @@
       <c r="D8" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="50" t="n">
+      <c r="E8" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F8" s="51" t="s">
         <v>219</v>
@@ -4885,9 +4917,9 @@
       <c r="D9" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="50" t="n">
+      <c r="E9" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F9" s="51" t="s">
         <v>219</v>
@@ -4917,9 +4949,9 @@
       <c r="D10" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="50" t="n">
+      <c r="E10" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F10" s="51" t="s">
         <v>219</v>
@@ -4951,9 +4983,9 @@
       <c r="D11" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="50" t="n">
+      <c r="E11" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F11" s="51" t="s">
         <v>219</v>
@@ -4978,14 +5010,12 @@
       <c r="A12" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B12"/>
-      <c r="C12"/>
       <c r="D12" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="50" t="n">
+      <c r="E12" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F12" s="51" t="s">
         <v>219</v>
@@ -4993,12 +5023,9 @@
       <c r="G12" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H12"/>
       <c r="I12" s="52">
         <v>5586076235</v>
       </c>
-      <c r="J12"/>
-      <c r="K12"/>
       <c r="L12" s="53" t="s">
         <v>51</v>
       </c>
@@ -5015,9 +5042,9 @@
       <c r="D13" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="50" t="n">
+      <c r="E13" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F13" s="51" t="s">
         <v>219</v>
@@ -5044,14 +5071,12 @@
       <c r="A14" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B14"/>
-      <c r="C14"/>
       <c r="D14" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="50" t="n">
+      <c r="E14" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F14" s="51" t="s">
         <v>219</v>
@@ -5059,12 +5084,9 @@
       <c r="G14" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H14"/>
       <c r="I14" s="52">
         <v>5586076235</v>
       </c>
-      <c r="J14"/>
-      <c r="K14"/>
       <c r="L14" s="53" t="s">
         <v>51</v>
       </c>
@@ -5076,14 +5098,12 @@
       <c r="A15" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B15"/>
-      <c r="C15"/>
       <c r="D15" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="50" t="n">
+      <c r="E15" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F15" s="51" t="s">
         <v>219</v>
@@ -5091,12 +5111,9 @@
       <c r="G15" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H15"/>
       <c r="I15" s="52">
         <v>6910855801</v>
       </c>
-      <c r="J15"/>
-      <c r="K15"/>
       <c r="L15" s="53" t="s">
         <v>51</v>
       </c>
@@ -5108,14 +5125,12 @@
       <c r="A16" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B16"/>
-      <c r="C16"/>
       <c r="D16" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="50" t="n">
+      <c r="E16" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F16" s="51" t="s">
         <v>219</v>
@@ -5123,12 +5138,9 @@
       <c r="G16" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H16"/>
       <c r="I16" s="52">
         <v>5586076235</v>
       </c>
-      <c r="J16"/>
-      <c r="K16"/>
       <c r="L16" s="53" t="s">
         <v>51</v>
       </c>
@@ -5145,9 +5157,9 @@
       <c r="D17" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="50" t="n">
+      <c r="E17" s="50">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F17" s="51" t="s">
         <v>219</v>
@@ -5172,14 +5184,12 @@
       <c r="A18" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B18"/>
-      <c r="C18"/>
       <c r="D18" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="50" t="n">
+      <c r="E18" s="50">
         <f ca="1">TODAY()</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F18" s="51" t="s">
         <v>219</v>
@@ -5187,12 +5197,9 @@
       <c r="G18" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H18"/>
       <c r="I18" s="52">
         <v>3341611017</v>
       </c>
-      <c r="J18"/>
-      <c r="K18"/>
       <c r="L18" s="53" t="s">
         <v>51</v>
       </c>
@@ -5204,14 +5211,12 @@
       <c r="A19" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B19"/>
-      <c r="C19"/>
       <c r="D19" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="50" t="n">
+      <c r="E19" s="50">
         <f ca="1">TODAY()</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F19" s="51" t="s">
         <v>219</v>
@@ -5219,12 +5224,9 @@
       <c r="G19" s="52">
         <v>8439809129</v>
       </c>
-      <c r="H19"/>
       <c r="I19" s="52">
         <v>3341611017</v>
       </c>
-      <c r="J19"/>
-      <c r="K19"/>
       <c r="L19" s="53" t="s">
         <v>51</v>
       </c>
@@ -5241,9 +5243,9 @@
       <c r="D20" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E20" s="50" t="n">
+      <c r="E20" s="50">
         <f ca="1">TODAY()</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F20" s="51" t="s">
         <v>219</v>
@@ -5273,9 +5275,9 @@
       <c r="D21" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="50" t="n">
+      <c r="E21" s="50">
         <f ca="1">TODAY()</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F21" s="51" t="s">
         <v>219</v>
@@ -5293,6 +5295,38 @@
         <v>51</v>
       </c>
       <c r="M21" s="54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="50">
+        <f ca="1">TODAY()</f>
+        <v>44389</v>
+      </c>
+      <c r="F22" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="G22" s="52">
+        <v>3426169660</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22" s="52">
+        <v>9849450932</v>
+      </c>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="M22" s="54" t="s">
         <v>107</v>
       </c>
     </row>
@@ -5302,53 +5336,189 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0D1CEF-B266-4241-89A5-652CE19CAC48}">
-  <dimension ref="A1:AH21"/>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F247C951-C76F-4C85-A12C-B9EAA29AC443}">
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="20" width="69.85546875" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" style="20" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="20" width="6.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="20" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="20" width="17.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="20" width="29.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="20" width="27.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="20" width="19.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="20" width="26.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="20" width="12.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="20" width="9.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="20" width="15.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="20" width="20.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="20" width="11.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="20" width="26.42578125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="20" width="18.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="20" width="21.140625" collapsed="true"/>
-    <col min="19" max="19" style="20" width="9.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="20" width="11.42578125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="20" width="13.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="20" width="11.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="20" width="8.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="20" width="12.5703125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="20" width="15.0" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="20" width="34.5703125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="20" width="12.85546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="20" width="16.7109375" collapsed="true"/>
-    <col min="29" max="29" style="20" width="9.140625" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="20" width="11.42578125" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="20" width="9.85546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="20" width="9.5703125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="20" width="8.140625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="20" width="12.0" collapsed="true"/>
-    <col min="35" max="16384" style="20" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0D1CEF-B266-4241-89A5-652CE19CAC48}">
+  <dimension ref="A1:AI22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="69.85546875" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="20" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.7109375" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.85546875" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.7109375" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27.42578125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="19.140625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.5703125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.28515625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.42578125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.140625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="26.42578125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="18.140625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="21.140625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="9.140625" style="20" collapsed="1"/>
+    <col min="21" max="21" width="11.42578125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.7109375" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.28515625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="8" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.5703125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="15" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="34.5703125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.85546875" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="16.7109375" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9.140625" style="20" collapsed="1"/>
+    <col min="31" max="31" width="11.42578125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.85546875" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="9.5703125" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="8.140625" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12" style="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="16384" width="9.140625" style="20" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5358,103 +5528,106 @@
       <c r="C1" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="G1" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="H1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="I1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="J1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="K1" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="L1" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="M1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="N1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="O1" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="P1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="Q1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="R1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="S1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="T1" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="U1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="V1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="30" t="s">
+      <c r="W1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="30" t="s">
+      <c r="X1" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="30" t="s">
+      <c r="Y1" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="30" t="s">
+      <c r="Z1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="30" t="s">
+      <c r="AA1" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="30" t="s">
+      <c r="AB1" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="30" t="s">
+      <c r="AC1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="30" t="s">
+      <c r="AD1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="30" t="s">
+      <c r="AE1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="30" t="s">
+      <c r="AF1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="30" t="s">
+      <c r="AG1" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="30" t="s">
+      <c r="AH1" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" s="30" t="s">
+      <c r="AI1" s="30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>98</v>
@@ -5462,47 +5635,49 @@
       <c r="C2" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="I2" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="J2" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="K2" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="L2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="M2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="21">
+      <c r="O2" s="21">
         <v>10</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="P2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="R2" s="21"/>
       <c r="S2" s="21"/>
       <c r="T2" s="21"/>
       <c r="U2" s="21"/>
@@ -5511,32 +5686,33 @@
       <c r="X2" s="21"/>
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
-      <c r="AA2" s="22" t="s">
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="AB2" s="21" t="s">
+      <c r="AC2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="AC2" s="21" t="s">
+      <c r="AD2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" s="21" t="s">
+      <c r="AE2" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="AE2" s="21" t="s">
+      <c r="AF2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="AF2" s="21" t="s">
+      <c r="AG2" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AG2" s="22" t="s">
+      <c r="AH2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="21" t="s">
+      <c r="AI2" s="21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>127</v>
       </c>
@@ -5546,37 +5722,46 @@
       <c r="C3" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E3" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="G3" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D4" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="72"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D5" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E5" s="72"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>199</v>
       </c>
@@ -5587,16 +5772,19 @@
         <v>98</v>
       </c>
       <c r="D6" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E6" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="G6" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>200</v>
       </c>
@@ -5607,16 +5795,19 @@
         <v>98</v>
       </c>
       <c r="D7" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="G7" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>201</v>
       </c>
@@ -5627,16 +5818,19 @@
         <v>98</v>
       </c>
       <c r="D8" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="G8" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>202</v>
       </c>
@@ -5647,16 +5841,19 @@
         <v>98</v>
       </c>
       <c r="D9" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="G9" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>203</v>
       </c>
@@ -5667,16 +5864,19 @@
         <v>98</v>
       </c>
       <c r="D10" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="G10" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>204</v>
       </c>
@@ -5687,16 +5887,19 @@
         <v>98</v>
       </c>
       <c r="D11" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="G11" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>140</v>
       </c>
@@ -5707,14 +5910,17 @@
         <v>98</v>
       </c>
       <c r="D12" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E12" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="G12" s="21"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>210</v>
       </c>
@@ -5725,34 +5931,43 @@
         <v>98</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="G13" s="21"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="D14" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E14" s="72"/>
       <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="G14" s="21"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E15" s="72"/>
       <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="G15" s="21"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>222</v>
       </c>
@@ -5763,14 +5978,17 @@
         <v>98</v>
       </c>
       <c r="D16" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E16" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>242</v>
       </c>
@@ -5781,14 +5999,17 @@
         <v>98</v>
       </c>
       <c r="D17" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E17" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>229</v>
       </c>
@@ -5799,14 +6020,17 @@
         <v>98</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E18" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>230</v>
       </c>
@@ -5817,14 +6041,17 @@
         <v>98</v>
       </c>
       <c r="D19" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>235</v>
       </c>
@@ -5835,14 +6062,17 @@
         <v>98</v>
       </c>
       <c r="D20" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E20" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>239</v>
       </c>
@@ -5853,12 +6083,36 @@
         <v>98</v>
       </c>
       <c r="D21" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E21" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5868,28 +6122,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAC3BBF-B3BA-44D1-A41A-B54909BFA2EB}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="10" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -5950,7 +6204,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>97</v>
@@ -6424,6 +6678,28 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
     </row>
+    <row r="22" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -6435,30 +6711,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6534BE01-4C47-4EFD-985F-408E3EBD759A}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="10" width="24.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="10" width="13.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="10" width="31.42578125" collapsed="true"/>
-    <col min="12" max="15" customWidth="true" style="10" width="13.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" style="10" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.42578125" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="15" width="13.140625" style="10" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -6528,7 +6804,7 @@
     </row>
     <row r="2" spans="1:21" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="11" t="str">
         <f>searchValues!D2</f>
@@ -6540,9 +6816,9 @@
       <c r="D2" s="29">
         <v>1075150626</v>
       </c>
-      <c r="E2" s="47" t="n">
+      <c r="E2" s="47">
         <f ca="1">searchValues!E2</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F2" s="47"/>
       <c r="G2" s="47"/>
@@ -6572,17 +6848,17 @@
       <c r="C3" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="29" t="n">
+      <c r="D3" s="29">
         <f>searchValues!I3</f>
-        <v>9.849450932E9</v>
-      </c>
-      <c r="E3" s="47" t="n">
+        <v>9849450932</v>
+      </c>
+      <c r="E3" s="47">
         <f ca="1">searchValues!E3</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F3" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F3" s="47">
         <f ca="1">searchValues!E3</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G3" s="47">
         <v>44696</v>
@@ -6618,9 +6894,9 @@
       <c r="D4" s="29">
         <v>1686560131</v>
       </c>
-      <c r="E4" s="47" t="n">
+      <c r="E4" s="47">
         <f ca="1">searchValues!E4</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47"/>
@@ -6653,13 +6929,13 @@
       <c r="D5" s="29">
         <v>1686560131</v>
       </c>
-      <c r="E5" s="47" t="n">
+      <c r="E5" s="47">
         <f ca="1">searchValues!E5</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F5" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F5" s="47">
         <f ca="1">searchValues!E5</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G5" s="47"/>
       <c r="H5" s="3"/>
@@ -6691,13 +6967,13 @@
       <c r="D6" s="29">
         <v>9564477390</v>
       </c>
-      <c r="E6" s="47" t="n">
+      <c r="E6" s="47">
         <f ca="1">searchValues!E6</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F6" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F6" s="47">
         <f ca="1">searchValues!E6</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G6" s="47">
         <v>44696</v>
@@ -6731,13 +7007,13 @@
       <c r="D7" s="29">
         <v>2011697620</v>
       </c>
-      <c r="E7" s="47" t="n">
+      <c r="E7" s="47">
         <f ca="1">searchValues!E7</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F7" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F7" s="47">
         <f ca="1">searchValues!E7</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G7" s="47">
         <v>44696</v>
@@ -6771,13 +7047,13 @@
       <c r="D8" s="29">
         <v>3941875192</v>
       </c>
-      <c r="E8" s="47" t="n">
+      <c r="E8" s="47">
         <f ca="1">searchValues!E8</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F8" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F8" s="47">
         <f ca="1">searchValues!E8</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G8" s="47">
         <v>44696</v>
@@ -6811,13 +7087,13 @@
       <c r="D9" s="29">
         <v>4086806378</v>
       </c>
-      <c r="E9" s="47" t="n">
+      <c r="E9" s="47">
         <f ca="1">searchValues!E9</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F9" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F9" s="47">
         <f ca="1">searchValues!E9</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G9" s="47">
         <v>44696</v>
@@ -6851,13 +7127,13 @@
       <c r="D10" s="29">
         <v>4030439314</v>
       </c>
-      <c r="E10" s="47" t="n">
+      <c r="E10" s="47">
         <f ca="1">searchValues!E10</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F10" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F10" s="47">
         <f ca="1">searchValues!E10</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G10" s="47">
         <v>44696</v>
@@ -6891,13 +7167,13 @@
       <c r="D11" s="29">
         <v>5012031479</v>
       </c>
-      <c r="E11" s="47" t="n">
+      <c r="E11" s="47">
         <f ca="1">searchValues!E11</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F11" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F11" s="47">
         <f ca="1">searchValues!E11</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G11" s="47">
         <v>44696</v>
@@ -6931,13 +7207,13 @@
       <c r="D12" s="29">
         <v>1272770452</v>
       </c>
-      <c r="E12" s="47" t="n">
+      <c r="E12" s="47">
         <f ca="1">searchValues!E12</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F12" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F12" s="47">
         <f ca="1">searchValues!E12</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G12" s="47">
         <v>44696</v>
@@ -6985,13 +7261,13 @@
       <c r="D13" s="29">
         <v>4172446499</v>
       </c>
-      <c r="E13" s="47" t="n">
+      <c r="E13" s="47">
         <f ca="1">searchValues!E13</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F13" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F13" s="47">
         <f ca="1">searchValues!E13</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G13" s="47">
         <v>44696</v>
@@ -7039,9 +7315,9 @@
       <c r="D14" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="E14" s="47" t="n">
+      <c r="E14" s="47">
         <f ca="1">searchValues!E14</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="F14" s="47">
         <v>44197</v>
@@ -7101,17 +7377,17 @@
       <c r="C15" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D15" s="29" t="n">
+      <c r="D15" s="29">
         <f>searchValues!I15</f>
-        <v>6.910855801E9</v>
-      </c>
-      <c r="E15" s="47" t="n">
+        <v>6910855801</v>
+      </c>
+      <c r="E15" s="47">
         <f ca="1">searchValues!E15</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F15" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F15" s="47">
         <f ca="1">searchValues!E15</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G15" s="47">
         <v>44696</v>
@@ -7156,17 +7432,17 @@
       <c r="C16" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="29" t="n">
+      <c r="D16" s="29">
         <f>searchValues!I16</f>
-        <v>5.586076235E9</v>
-      </c>
-      <c r="E16" s="47" t="n">
+        <v>5586076235</v>
+      </c>
+      <c r="E16" s="47">
         <f ca="1">searchValues!E16</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F16" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F16" s="47">
         <f ca="1">searchValues!E16</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G16" s="47"/>
       <c r="H16" s="3"/>
@@ -7195,17 +7471,17 @@
       <c r="C17" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D17" s="29" t="n">
+      <c r="D17" s="29">
         <f>searchValues!I17</f>
-        <v>5.586076235E9</v>
-      </c>
-      <c r="E17" s="47" t="n">
+        <v>5586076235</v>
+      </c>
+      <c r="E17" s="47">
         <f ca="1">searchValues!E17</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F17" s="47" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F17" s="47">
         <f ca="1">searchValues!E17</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G17" s="47"/>
       <c r="H17" s="3"/>
@@ -7232,17 +7508,17 @@
         <v>Personal Auto</v>
       </c>
       <c r="C18" s="11"/>
-      <c r="D18" s="64" t="n">
+      <c r="D18" s="64">
         <f>searchValues!I18</f>
-        <v>3.341611017E9</v>
-      </c>
-      <c r="E18" s="47" t="n">
-        <f t="shared" ref="E18:F21" ca="1" si="0">TODAY()</f>
-        <v>44384.0</v>
-      </c>
-      <c r="F18" s="47" t="n">
+        <v>3341611017</v>
+      </c>
+      <c r="E18" s="47">
+        <f t="shared" ref="E18:F22" ca="1" si="0">TODAY()</f>
+        <v>44389</v>
+      </c>
+      <c r="F18" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G18" s="47"/>
       <c r="H18" s="3"/>
@@ -7271,17 +7547,17 @@
       <c r="C19" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D19" s="3" t="n">
+      <c r="D19" s="3">
         <f>searchValues!I19</f>
-        <v>3.341611017E9</v>
-      </c>
-      <c r="E19" s="65" t="n">
+        <v>3341611017</v>
+      </c>
+      <c r="E19" s="65">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
-      </c>
-      <c r="F19" s="65" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F19" s="65">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -7310,17 +7586,17 @@
       <c r="C20" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="3">
         <f>searchValues!I20</f>
-        <v>9.849450932E9</v>
-      </c>
-      <c r="E20" s="65" t="n">
+        <v>9849450932</v>
+      </c>
+      <c r="E20" s="65">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
-      </c>
-      <c r="F20" s="65" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F20" s="65">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -7349,17 +7625,17 @@
       <c r="C21" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="3">
         <f>searchValues!I21</f>
-        <v>9.849450932E9</v>
-      </c>
-      <c r="E21" s="65" t="n">
+        <v>9849450932</v>
+      </c>
+      <c r="E21" s="65">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
-      </c>
-      <c r="F21" s="65" t="n">
+        <v>44389</v>
+      </c>
+      <c r="F21" s="65">
         <f t="shared" ca="1" si="0"/>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -7377,6 +7653,45 @@
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
     </row>
+    <row r="22" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="3" t="str">
+        <f>searchValues!D22</f>
+        <v>Personal Auto</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="3">
+        <f>searchValues!I22</f>
+        <v>9849450932</v>
+      </c>
+      <c r="E22" s="65">
+        <f t="shared" ca="1" si="0"/>
+        <v>44389</v>
+      </c>
+      <c r="F22" s="65">
+        <f t="shared" ca="1" si="0"/>
+        <v>44389</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7388,13 +7703,13 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7410,7 +7725,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -7561,29 +7876,31 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C4E6E2-AAC9-4B7B-B879-C23DF8988E6C}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="66.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="10" width="18.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="21.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="10" width="21.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.28515625" style="10" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21" style="10" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="31.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -7629,20 +7946,38 @@
       <c r="O1" s="31" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
@@ -7688,13 +8023,25 @@
       <c r="O4" s="10">
         <v>46074</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>140</v>
       </c>
@@ -7713,8 +8060,14 @@
       <c r="O6" s="10">
         <v>46074</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>141</v>
       </c>
@@ -7760,8 +8113,14 @@
       <c r="O7" s="10">
         <v>46074</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>142</v>
       </c>
@@ -7779,6 +8138,12 @@
       </c>
       <c r="O8" s="10">
         <v>46074</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -7792,13 +8157,13 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="66.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7817,7 +8182,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" s="44"/>
     </row>
@@ -7877,21 +8242,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBAA54D-4167-4FED-9056-FD7F72E35B94}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="69.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -7919,14 +8284,14 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="34" t="n">
+      <c r="C2" s="34">
         <f ca="1">TODAY()</f>
-        <v>44384.0</v>
+        <v>44389</v>
       </c>
       <c r="D2" s="34">
         <v>44706</v>
@@ -8034,6 +8399,11 @@
     <row r="21" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>